<commit_message>
finalisation ajout articles manuels
</commit_message>
<xml_diff>
--- a/Datasets/GameSE/tmp manuel.xlsx
+++ b/Datasets/GameSE/tmp manuel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udemontreal-my.sharepoint.com/personal/guillaume_genois_umontreal_ca/Documents/Projet Curation des métadonnées/Datasets/GameSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="11_F25DC773A252ABDACC10482D419A5A3A5ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC40C414-C368-4C56-9E0E-F4613EBD656F}"/>
+  <xr:revisionPtr revIDLastSave="463" documentId="11_F25DC773A252ABDACC10482D419A5A3A5ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3901FEF3-67A8-456C-82BB-AA15D8CDB1B1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="459">
   <si>
     <t>key</t>
   </si>
@@ -1106,6 +1106,373 @@
   </si>
   <si>
     <t>Extrait</t>
+  </si>
+  <si>
+    <t>I have a problem: it’s called preaching to the choir.  Nobody here lacks faith in the history of games, and I can only hope that my talk will not reduce your enthusiasm.  That realization eliminates the need for a homily on the value of historical studies.  Instead, I will talk about the possibilities and promises facing the history of games as we plunge forward. What does history offer game studies and what might a history of games give back? These questions guide my thoughts at the end of this conference, which has given so much food for these thoughts.</t>
+  </si>
+  <si>
+    <t>History of Games International Conference Proceedings</t>
+  </si>
+  <si>
+    <t>https://www.kinephanos.ca/2014/game-engines-and-game-history/</t>
+  </si>
+  <si>
+    <t>Lowood, Henry</t>
+  </si>
+  <si>
+    <t>Kinephanos</t>
+  </si>
+  <si>
+    <t>https://odr.chalmers.se/items/d5fe6889-4cc6-49c2-ba56-0d759e2f37eb</t>
+  </si>
+  <si>
+    <t>Fagerholt, Erik; Lorentzon, Magnus</t>
+  </si>
+  <si>
+    <t>Datalogi; Bildanalys; Computer science; Image analysis</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/prov-primer/</t>
+  </si>
+  <si>
+    <t>This document provides an intuitive introduction and guide to the PROV Data Model for provenance interchange on the web. PROV defines a core data model for provenance for building representations of the entities, people and processes involved in producing a piece of data or thing in the world. This primer explains the fundamental PROV concepts and provides examples of its use. The primer is intended as a starting point for those wishing to create or use PROV data.
+The PROV Document Overview describes the overall state of PROV, and should be read before other PROV documents.</t>
+  </si>
+  <si>
+    <t>Gil, Yolanda; Miles, Simon; Belhajjame, Khalid; Deus, Helena F.; Garijo, Daniel; Klyne, Graham; Missier, Paolo; Soiland-Reyes, Stian; Zednik, Stephan</t>
+  </si>
+  <si>
+    <t>Reliability; Validity; Triangulation; Construct; Qualitative; Quantitative</t>
+  </si>
+  <si>
+    <t>The use of reliability and validity are common in quantitative research and now it is reconsidered in the qualitative research paradigm. Since reliability and validity are rooted in positivist perspective then they should be redefined for their use in a naturalistic approach. Like reliability and validity as used in quantitative research are providing springboard to examine what these two terms mean in the qualitative research paradigm, triangulation as used in quantitative research to test the reliability and validity can also illuminate some ways to test or maximize the validity and reliability of a qualitative study. Therefore, reliability, validity and triangulation, if they are relevant research concepts, particularly from a qualitative point of view, have to be redefined in order to reflect the multiple ways of establishing truth.</t>
+  </si>
+  <si>
+    <t>597-606</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.46743/2160-3715/2003.1870</t>
+  </si>
+  <si>
+    <t>Work for Play: Careers in Video Game Development</t>
+  </si>
+  <si>
+    <t>Video games are not only for play; they also provide work. Making video games is a serious--and big--business. Creating these games is complex and requires the collaboration of many developers, who perform a variety of tasks, from production to programming. They work for both small and large game studios to create games that can be played on many different devices, including console systems, computers, and cell phones. This article covers career options in video game development. The first section provides an overview of the development process. The second section describes four groups of video game occupations: designers, programmers, artists, and others. The third section covers the skills and training workers need for these jobs. The fourth section discusses the benefits and challenges of working in the video game industry. And the fifth section provides job-seeking tips for a career in video game development. Suggested resources for additional information are presented.</t>
+  </si>
+  <si>
+    <t>Video Games; Development; Occupational Information; Employment Opportunities; Employment Qualifications; Educational Attainment</t>
+  </si>
+  <si>
+    <t>Liming, Drew; Vilorio, Dennis</t>
+  </si>
+  <si>
+    <t>Occupational Outlook Quarterly</t>
+  </si>
+  <si>
+    <t>https://eric.ed.gov/?id=EJ945968</t>
+  </si>
+  <si>
+    <t>2-11</t>
+  </si>
+  <si>
+    <t>Purpose
+This paper aims to present a new approach for developing a framework based on a model driven architecture (MDA) for the modelling of technology‐independent collaborative processes.
+Design/methodology/approach
+The paper suggests a new collaborative process modelling approach based on an MDA and a metamodelling technique. The research method, based on the design science approach, was started by identifying the characteristics of the collaborative processes, which distinguish them from the classical intraorganizational ones. Then, the generic collaborative business process (CBP) modelling framework is developed based on MDA approach and definition of a set of transformation rules through three layers: business, process, and technical. After that, the core component of the framework was the proposition of a generic CBP metamodel at PIM/MDA level. The specific collaboration participant's business processes (expressed as BPMN model) are generated from the generic CBP model represented as an UML2 Profile activity diagram, which is compliant to CBP metamodel. Finally, as proof‐of‐concept, the architecture of an Eclipse‐based open development platform is developed implementing an e‐Procurement collaborative process.
+Findings
+The proposed framework for CBP modelling and the generic CBP metamodel contribute towards a more efficient methodology and have consequences for BPM‐related collaboration, facilitating the B2B processes modelling and implementation. In order to demonstrate and evaluate the practical applicability of the framework, the architecture of an Eclipse‐based open development platform is developed implementing a collaborative business application on the basis of an e‐Procurement use case.
+Research limitations/implications
+There is a need to focus future research efforts on the improvement of the semi‐automatic transformation phase from public to private processes which needs human intervention by adding a suitable interfaces at both sides of the B2B interaction. In addition, the problem of semantic heterogeneities regarding the partner's business process elements (business documents, activity/task names) should be tackled by developing an approach that uses ontology.
+Practical implications
+Business processes developers find a B2B technology‐independent solution for implementing and using interorganizational information systems.
+Originality/value
+The paper provides a framework that enables the CBP modelling and integrates a generic CBP metamodel. Currently, to the best of the authors' knowledge, such a generic metamodel and his instantiation have not so far been developed.</t>
+  </si>
+  <si>
+    <t>An MDA‐based framework for collaborative business process modelling</t>
+  </si>
+  <si>
+    <t>Business process; Collaborative business process; Collaborative business process metamodel; MDA-based framework; E-procurement; UML2 profile; Process management; Team working</t>
+  </si>
+  <si>
+    <t>Bouchbout, Khoutir; Akoka, Jacky; Alimazighi, Zaia</t>
+  </si>
+  <si>
+    <t>https://www.emerald.com/insight/content/doi/10.1108/14637151211283357/full/html?casa_token=mpPxdAoPSnQAAAAA:TadUnDgj7LnKG7kXx7SeBjOLPyTCUMWeAl9efrrDz4b-T4P5hD6H5anWd4q3eZ-zln_1ER4uuIYL5fthV_hpBHGldsU-nCFmOWZ127H6UxvmwRMvgDTL6w</t>
+  </si>
+  <si>
+    <t>Emerald Insight</t>
+  </si>
+  <si>
+    <t>IGI Global Reasearch</t>
+  </si>
+  <si>
+    <t>https://www.igi-global.com/chapter/design-play-experience-framework/20133</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.4018/978-1-59904-808-6.CH058</t>
+  </si>
+  <si>
+    <t>This chapter introduces a framework for the design of serious games for learning, called the design, play, and experience framework. The author argues that the great potential of serious games will not be realized without a formal design approach. To that end, the author presents and thoroughly explains the design, play, and experience framework which provides a formal approach to designing the learning, storytelling, game play, user experience, and technology components of a serious game. The author concludes by detailing how the framework provides a common language to discuss serious game design, a methodology to analyze a design, and a process to design a serious game for learning.</t>
+  </si>
+  <si>
+    <t>Prototyping; Serious Games; Iterative Game Design; Heart of Serious Game Design; Exogenous Educational Games; Balancing; Endogenous Educational Games; Game Design; Game Mechanics; Game Dynamics</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Comparison of a Traditional and a Video Game Based Balance Training Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The aim of the present study is to compare the efficiency of traditional and video game based balance training programs. 22 customers of a health care
+centre (age: M = 47.6 yrs; SD = 13.1) volunteered to participate in the experiment. They were randomly assigned to two experimental groups. One group underwent a traditional training program, while the other group trained using the Nintendo Wii Fit TM Balance Board. Between pre and post test procedures, training sessions were performed three times a week for three weeks. In addition to five balance tests (SEBT, ball-handling, two video games, dynamic balance), a questionnaire was applied concerning mood state, self-efficacy, physical activity enjoyment, flow and subjective experience in order to evaluate psychological effects of the interventions. Two-factor analyses of variance showed both general and differential improvements of the two groups for pre and post test measures. Both groups improved their balance performance in 4 of five tests. The traditional group showed a significantly greater improvement in two tests (SEBT: F(1,20) = 8.907, p = .007, η2 = .308; ball-handling: F(1,20) = 13.578, p = .001, η2 = .404),
+whereas the Wii group showed a significantly greater improvement in one test (Ski Slalom (F(1,20) = 5.101, p = .035, η2 = .203). Psychological questionnaires revealed neither significant pre-post effects nor differences between the groups for pre and post test measurements. The results confirm that the Nintendo Wii Fit TM may be a suitable medium
+of training balance in prevention and rehabilitation of adults. Specific effects of training are more pronounced than transfer between virtual and real performance. </t>
+  </si>
+  <si>
+    <t>BALANCE; VIDEO GAMES; NINTENDO Wii Fit TM; REHABILITATION; PREVENTION</t>
+  </si>
+  <si>
+    <t>International Journal of Computer Science in Sport</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Josef-Wiemeyer/publication/220244895_Comparison_of_a_traditional_and_a_Video_Game_Based_Balance_Training_Program/links/54806fad0cf25b80dd723663/Comparison-of-a-traditional-and-a-Video-Game-Based-Balance-Training-Program.pdf</t>
+  </si>
+  <si>
+    <t>Kliem, Annika; Wiemeyer, Josef</t>
+  </si>
+  <si>
+    <t>IACSS</t>
+  </si>
+  <si>
+    <t>https://aisel.aisnet.org/jais/vol11/iss11/2/</t>
+  </si>
+  <si>
+    <t>Association for Information Systems</t>
+  </si>
+  <si>
+    <t>Alspaugh, Thomas A.; Scacchi, Walt; Asuncion, Hazeline U.</t>
+  </si>
+  <si>
+    <t>The prevailing approach to free/open source software and licenses has been that each system is developed, distributed, and used under the terms of a single license. But it is increasingly common for information systems and other software to be composed with components from a variety of sources, and with a diversity of licenses. This may result in possible license conflicts and organizational liability for failure to fulfill license obligations. Research and practice to date have not kept up with this sea-change in software licensing arising from free/open source software development. System consumers and users consequently rely on ad hoc heuristics (or costly legal advice) to determine which license rights and obligations are in effect, often with less than optimal results; consulting services are offered to identify unknowing unauthorized use of licensed software in information systems; and researchers have shown how the choice of a (single) specific license for a product affects project success and system adoption. Legal scholars have examined how pairs of software licenses conflict but only in simple contexts. We present an approach for understanding and modeling software licenses, as well as for analyzing conflicts among groups of licenses in realistic system contexts, and for guiding the acquisition, integration, or development of systems with free/open source components in such an environment. This work is based on an empirical analysis of representative software licenses and of heterogeneously-licensed systems. Our approach provides guidance for achieving a “best-of-breed” component strategy while obtaining desired license rights in exchange for acceptable obligations.</t>
+  </si>
+  <si>
+    <t>game design; design tools; ludocore; machinations; game atoms; game diagramming</t>
+  </si>
+  <si>
+    <t>The art form of the video game has a very idiosyncratic reliance on the process and practice of its designers. We work with creative and computational problems that form a web of deep complexity. And yet, as I have noticed in my professional practice as a game designer, we do not use tools to support our design process. For more than a decade, designers and researchers have argued for the development and use of both conceptual and concrete tools. To this end, formal and semi-formal game design models have been proposed and, more recently, experimental software-based tools have been developed by the research community. To date, however, none of these tools or models have been adopted into mainstream practice within the game design community. In this paper I argue that it is difficult, if not methodologically flawed, to assess the work in the field of game design support without more qualitative data on how such tools fare in actual game design practice. Evaluation research would be an essential contribution towards answering the question of whether – and if so, how - these experimental formal models and tools can support and improve the game design process.</t>
+  </si>
+  <si>
+    <t>Game design tools: Time to evaluate</t>
+  </si>
+  <si>
+    <t>Proceedings of Nordic DiGRA 2012 Conference</t>
+  </si>
+  <si>
+    <t>https://dl.digra.org/index.php/dl/article/view/606</t>
+  </si>
+  <si>
+    <t>@Conference{digra606, title ="Game design tools: Time to evaluate", year = "2012", author = "Neil, Katharine", publisher = "DiGRA", address = "Tampere", howpublished = "\url{https://dl.digra.org/index.php/dl/article/view/606}", booktitle = "Proceedings of Nordic DiGRA 2012 Conference"}</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/1461444809342738</t>
+  </si>
+  <si>
+    <t>The politics of ‘platforms’</t>
+  </si>
+  <si>
+    <t>Online content providers such as YouTube are carefully positioning themselves to users, clients, advertisers and policymakers, making strategic claims for what they do and do not do, and how their place in the information landscape should be understood. One term in particular, ‘platform’, reveals the contours of this discursive work. The term has been deployed in both their populist appeals and their marketing pitches, sometimes as technical ‘platforms’, sometimes as ‘platforms’ from which to speak, sometimes as ‘platforms’ of opportunity. Whatever tensions exist in serving all of these constituencies are carefully elided. The term also fits their efforts to shape information policy, where they seek protection for facilitating user expression, yet also seek limited liability for what those users say. As these providers become the curators of public discourse, we must examine the roles they aim to play, and the terms by which they hope to be judged.</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/10.1177/1461444809342738</t>
+  </si>
+  <si>
+    <t>Sage Journals</t>
+  </si>
+  <si>
+    <t>New Media &amp; Society</t>
+  </si>
+  <si>
+    <t>Usability of Web sites, methods and evaluation techniques</t>
+  </si>
+  <si>
+    <t>In the present society, the relevance of the Web is unquestionable and there is a great variety of Web sites that offer services to users. In this context, usability plays a fundamental role in the process of developing successful Web sites. In this article we review different definitions about the discipline of usability, its incorporation in the engineering process (usability engineering) and its relation to software engineer, as well as its attributes and evaluation methods. The considerations about the evaluation system of the Web usability are also presented, advising the user and basing it in the establishment of critical tasks (SIRIUS, reviewed by the authors).</t>
+  </si>
+  <si>
+    <t>Web site; usability; usability evaluation; heuristic; expert; classification of Web sites; Web tools</t>
+  </si>
+  <si>
+    <t>Jaimes, Oscar Mauricio Serrano; Gonzalez, Carlos Alberto Rodriguez; de Sistemas, Ingeniero</t>
+  </si>
+  <si>
+    <t>Revista Cubana de Información en Ciencias de la Salud</t>
+  </si>
+  <si>
+    <t>http://scielo.sld.cu/scielo.php?script=sci_arttext&amp;pid=S2307-21132013000200007</t>
+  </si>
+  <si>
+    <t>Due to the recent proliferation of free-to-use, professional-quality development tools, crowdsourced fundraising, and the ascendency of digital distribution platforms, ‘indie’ digital game developers are emerging on an unprecedented scale. Based on ethnographic research conducted at indie accelerator Execution Labs from January to June of 2015, this thesis explores how indie developers frame risk, creativity, success, and failure in relation to the communities they are a part of. The first three chapters highlight useful concepts from Gina Neff’s ‘Venture Labour’ (2012), describe Execution Labs from the researcher’s perspective, and detail the researcher’s approach to collaborative embedded ethnography, respectively. The fourth chapter is dedicated to two related purposes: the first part will posit that communities of indie developers and indie fans share a common creative discourse, and thus constitute what Benedict Anderson has termed an ‘Imagined Community’ (2006). The latter portion of the chapter will explore how Newgrounds.com facilitated discourses about digital games and Macromedia Flash, and how the resultant imagined communities have influenced contemporary indie identity and development practice. The final chapter opens by proposing a definition of ‘indie labour’: a creative, communitarian strategy with which indie developers manage the risks they face. It will then consider the stories of those who performed indie labour as part of Execution Labs. This thesis will conclude by ruminating on potential future avenues of study and ongoing issues that hinder indie development’s potential as an open and accessible praxis.</t>
+  </si>
+  <si>
+    <t>Communication Studies</t>
+  </si>
+  <si>
+    <t>Concordia University</t>
+  </si>
+  <si>
+    <t>https://spectrum.library.concordia.ca/id/eprint/980737/</t>
+  </si>
+  <si>
+    <t>https://repositorio-aberto.up.pt/bitstream/10216/91011/2/176444.pdf</t>
+  </si>
+  <si>
+    <t>Manuel António da Cruz Lopes</t>
+  </si>
+  <si>
+    <t>Computer games have a long tradition in the Artificial Intelligence (AI) field. They serve the purpose of establishing challenging goals with long term positive repercussions, with researchers trying to develop AIs capable of beating the world human experts. They also provide a good amount of exposition in mainstream media, whilst also giving an engaging environment for teaching computer science concepts in general and AI methods in particular. This thesis aims precisely to contribute to the educational gaming landscape, by providing a novel Bomberman themed platform and several associated intelligent agents. Our first major contribution is precisely the platform itself, Bomberman
+as an Artificial Intelligence Platform (BAIP). We provide a fully functional opensource, graphical, language agnostic platform, aimed towards facilitating the study and development of AI methods. We showcase the potential of BAIP and the richness of the selected game environment by developing a plethora of AI agents using different methodologies. At an initial level we introduce a set of basic heuristic methods capable of providing agents with the most essential behavior primitives, equipping them for basic survival in the game environment. At a more advanced level we introduce search-based methods capable of some form of planning. From a machine learning perspective we show how BAIP can be integrated and used with Reinforcement Learning (RL). We use a simple RL problem within the platform and implement both Q-learning and Sarsa algorithms in order to tackle it. This thesis also provides detailed and thorough experimental results about all the developed agents and methods, using the developed platform capabilities. To sum up, this work introduces a new AI platform, gives a strong baseline agent and demonstrates the feasibility of using it for machine learning tasks.</t>
+  </si>
+  <si>
+    <t>Faculdade de Ciencias da Universidade do Porto</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.17487/RFC5905</t>
+  </si>
+  <si>
+    <t>The Network Time Protocol (NTP) is widely used to synchronize computer clocks in the Internet. This document describes NTP version 4 (NTPv4), which is backwards compatible with NTP version 3 (NTPv3), described in RFC 1305, as well as previous versions of the protocol. NTPv4 includes a modified protocol header to accommodate the Internet Protocol version 6 address family. NTPv4 includes fundamental improvements in the mitigation and discipline algorithms that extend the potential accuracy to the tens of microseconds with modern workstations and fast LANs. It includes a dynamic server discovery scheme, so that in many cases, specific server configuration is not required. It corrects certain errors in the NTPv3 design and implementation and includes an optional extension mechanism. [STANDARDS-TRACK]</t>
+  </si>
+  <si>
+    <t>Mills, D.; J. Martin, Ed.; Burbank, J.; Kasch, W.</t>
+  </si>
+  <si>
+    <t>RFC Editor</t>
+  </si>
+  <si>
+    <t>From Knowing It to “Getting It”: Envisioning Practices in Computer Games Development</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1287/isre.2013.0482</t>
+  </si>
+  <si>
+    <t>https://pubsonline.informs.org/doi/10.1287/isre.2013.0482</t>
+  </si>
+  <si>
+    <t>Nandhakumar, Joe; Panourgias, Nikiforos S.; Scarbrough, Harry</t>
+  </si>
+  <si>
+    <t>Information Systems Research</t>
+  </si>
+  <si>
+    <t>collaborative practice; envizioning; interpretive; computer games development; emergence</t>
+  </si>
+  <si>
+    <t>The development of information systems and software applications increasingly needs to deliver culturally rich and affective experiences for user groups. In this paper, we explore how the collaborative practices across different expert groups can enable this experiential dimension of use to be integrated into the development of a software product. In an empirical study of computer games development—an arena in which the novelty and richness of the user experience is central to competitive success—we identify the challenges of conceptualizing and realizing a desired user experience when it cannot be readily specified in an initial design template, nor represented within the expertise of existing groups. Our study develops a theoretical framework to address these challenges. Through this framework, we are able to show how achieving a desired user experience requires developer groups to not only work across the boundaries that arise from specialized expertise, but also across wider fields centred on cultural production and software development, respectively. We find that their ability to do this is supported by distinctive “envisioning practices” that sustain an emerging shared “vision” for each game. The key research contributions that we then make are (a) grounding envisioning practices as a means of theorizing the collaborative practices centred on conceptualizing the user experience; (b) identifying how these practices are interwoven with the “producing practices” of software development, thus enabling collaboration to span expert groups and disparate fields; and (c) theorizing the role of vision as an emerging conceptual boundary object in these practices.</t>
+  </si>
+  <si>
+    <t>933-955</t>
+  </si>
+  <si>
+    <t>https://www.rfc-editor.org/info/rfc5905</t>
+  </si>
+  <si>
+    <t>Institute for Operations Research and the Management Sciences</t>
+  </si>
+  <si>
+    <t>Controlling the uncontrollable: ‘Agile’ teams and illusions of autonomy in creative work</t>
+  </si>
+  <si>
+    <t>The creative industries have recently been hailed as presenting a liberating model for the future of work and a valuable terrain on which to examine purported new regimes of workplace control. This article, based on the empirical examination of a Canadian video game development studio, traces the modes of control which operate on and through project teams in creative settings. The impact of the adoption of an ‘emancipatory’, post-bureaucratic project management technology, ‘Agile’, is critically examined through interviews and non-participative observation of management, technical and artistic labour within one project team. The potential for autonomy in such ‘Agile’ teams is critically assessed within the managerial regime of creative production and the broader power relations implied by the financial, organizational and institutional context.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/0950017012460315</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/full/10.1177/0950017012460315?casa_token=G-C_d0fPy78AAAAA%3Ayy58QtV0Slb683uh32WHxvq99ydiee92W1YtKcnNS66g2zzSjw2H44cE8Y8D9oZ6QJXlDUugspYDymo</t>
+  </si>
+  <si>
+    <t>Hodgson, Damian; Briand, Louise</t>
+  </si>
+  <si>
+    <t>Requirement Engineering (RE) plays an important role in the success of software development life cycle. As RE is the starting point of the life cycle, any changes in requirements will be costly and time consuming. Failure in determining accurate requirements leads to errors in specifications and therefore to a mal system architecture. In addition, most of software development environments are characterized by user requests to change some requirements.Scrum as one of agile development methods that gained a great attention because of its ability to deal with the changing environments. This paper presents and discusses the current situation of RE activities in Scrum, how Scrum benefits from RE techniques and future challenges in this respect.</t>
+  </si>
+  <si>
+    <t>Agile; Requirement Engineering; Software Development; Scrums</t>
+  </si>
+  <si>
+    <t>Darwish, Nagy Ramadan; Megahed, Salwa</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Nagy-Ramadan/publication/308186449_Requirements_Engineering_in_Scrum_Framework/links/57de46b008aeea195938d140/Requirements-Engineering-in-Scrum-Framework.pdf</t>
+  </si>
+  <si>
+    <t>International Journal of Computer Applications</t>
+  </si>
+  <si>
+    <t>Foundation of Computer Science</t>
+  </si>
+  <si>
+    <t>Software in 30 days: how agile managers beat the odds, delight their customers, and leave competitors in the dust</t>
+  </si>
+  <si>
+    <t>https://books.google.ca/books?hl=en&amp;lr=&amp;id=FSQbYl5HMo8C&amp;oi=fnd&amp;pg=PP11&amp;dq=Software+in+30+Days:+How+Agile+Managers+Beat+the+Odds,+Delight+Their+Customers,+And+Leave+Competitors+In+the+Dust+-+The+Scrum+Guide&amp;ots=V6fElsfP-i&amp;sig=1MZtgdg3yY7QYqedHD2x_gdHmTU#v=onepage&amp;q=Software%20in%2030%20Days%3A%20How%20Agile%20Managers%20Beat%20the%20Odds%2C%20Delight%20Their%20Customers%2C%20And%20Leave%20Competitors%20In%20the%20Dust%20-%20The%20Scrum%20Guide&amp;f=false</t>
+  </si>
+  <si>
+    <t>Schwaber, Ken; Sutherland, Jeff</t>
+  </si>
+  <si>
+    <t>This article aims at characterizing the Danish Christmas calendar as a TV institution and a meeting place for the traditions of the almanac, folklore and the history of culture. Against the background of a brief outline of the history of Danish Christmas calendars, the article explores ways in which this traditional genre has succeeded in renewing itself. The so-called Pyrus series, TV 2’s Christmas calendars during the mid-1990s, exhibited folklore, myth and cultural history in a combination of entertainment and information. They were succeeded by calendars such as Jul i Valhal/‘Christmas in Valhalla’ (2005), Absalons hemmelighed/‘The Secret of Absalon’ (2006), Mikkel og guldkortet/‘Mikkel and the Golden Card’ (2008) and Pagten/‘The Covenant’ (2009). Some of these added cultural criticism to the repertoire of the genre.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1386/jsca.3.3.267_1</t>
+  </si>
+  <si>
+    <t>267 - 280</t>
+  </si>
+  <si>
+    <t>https://intellectdiscover.com/content/journals/10.1386/jsca.3.3.267_1</t>
+  </si>
+  <si>
+    <t>Intellect Discover</t>
+  </si>
+  <si>
+    <t>We, Jeff and Ken, have been in the software industry, collectively, for 70 years. We have been software developers, managers in IT organizations and software product companies, and owners of both product companies and service organizations. More than 20 years ago, we created a process that lets organizations deliver software better. Since then, we have helped hundreds of organizations do the same. Our work has spread further than we have ever imagined possible, being put to use by millions of people. We are humbled by the extent of its adoption, and we are awed by the feats people have accomplished using it. This is not the first book we have written on the topic of building software. It is, however, the first book we have written for people who do not themselves build software. This book is instead for leaders within organizations that depend on software for their survival and competitiveness. It is for leaders within organizations that can benefit from developing software rapidly, inerementally. and with the best return on investment possible. It is for leaders who face business and technological complexity that has made the delivery of software difficult. We have written this book so that these leaders can help their organizations achieve these goals, enhance their internal capabilities, improve their product offerings, and more. This book is for chief executive officers (CEOs), executives, and senior managers who need their organizations to deliver better software in less time, with lower cost, greater predictability, and lower risk. For this audience, we have a message: You may have had negative experiences with software devel- opment in the past, but the industry has turned a corner. The software profes- sion has radically improved its methods and its results. The uncertainty, risk, and waste to which you are accustomed are no longer par for the course. We have worked with many software organizations that have already turned the corner; we want to help you do so, too. In this book, we show you how to create business value using a process that delivers complete pieces of software functionality at least every 30 days. This book will show you how you can prioritize the functionality you want and have it delivered á la carte. It will show you how to gain transparency not only into business value, by tracking functionality delivered against functionality desired, but also into the health of the software development process and your organization as a whole. The tools in this book will help you work with your software organization to get up to speed with modern practices and begin to deliver the results you've been expecting all along. This is software in 30 days.</t>
+  </si>
+  <si>
+    <t>https://gamestudies.org/1001/articles/mayra</t>
+  </si>
+  <si>
+    <t>Gaming Culture at the Boundaries of Play</t>
+  </si>
+  <si>
+    <t>As the field of game studies and research has matured, multiple valid, yet somewhat differently oriented approaches to games, play and players have emerged. One of them is the cultural study of games and play related phenomena. Both the British and American traditions of cultural studies have been particularly interested in advancing our understanding of popular culture by tracing its position and significance from perspectives opened up by politics, economics, sociology, as well as by literary or textual studies, to mention just a few elements from this highly interdisciplinary field. Where the hallmark of British cultural studies used to be reliance on some version of Marxism or left-wing critique of capitalist society and its cultural industries, and the American approach to cultural studies was more likely to develop liberalist analyses of empowered audiences, or fandom activities, this divide does not stand out so clearly these days. While approaching Cheating by Mia Consalvo, it is nevertheless useful to be keep in mind such intellectual traditions and debates.</t>
+  </si>
+  <si>
+    <t>Frans Mäyrä</t>
+  </si>
+  <si>
+    <t>Dit proefschrift presenteert twee theoretische kaders voor het ontwerpen van games en beschrijft hoe game designers deze kunnen inzetten om het game ontwerpproces te stroomlijnen. Er bestaan op dit moment meerdere ontwerptheorie¨en voor games, maar geen enkele kan rekenen op een breed draagvlak binnen de game industrie. Vooral academische ontwerptheorie¨en hebben regelmatig een slechte reputatie. Het eerste kader dat game designers inzicht biedt in spelregels en hun werking heet Machinations en maakt gebruik van dynamische, interactieve diagrammen. Het tweede theoretische kader van dit proefschrift, Mission/Space, richt zich op level-ontwerp en spelmechanismen die de voortgang van een speler bepalen. In tegenstelling tot bestaande modellen voor level-ontwerp, bouwt Mission/Space voort op het idee dat er in een level twee verschillende structuren bestaan. Mission-diagrammen worden gebruikt om de structuur van taken en uitdagingen voor de speler te formaliseren, terwijl space-diagrammen de ruimtelijke constructie formaliseren. Beide constructies zijn aan elkaar gerelateerd, maar zijn niet hetzelfde. De verschillende wijzen waarop missies geprojecteerd kunnen worden op een bepaalde ruimte speelt uiteindelijk een belangrijke rol in de totstandkoming van de spelervaring.</t>
+  </si>
+  <si>
+    <t>The Free Lunch Is Over: A Fundamental Turn Toward Concurrency in Software</t>
+  </si>
+  <si>
+    <t>Your free lunch will soon be over. What can you do about it? What are you doing about it? The major processor manufacturers and architectures, from Intel and AMD to Sparc and PowerPC, have run out of room with most of their traditional approaches to boosting CPU performance. Instead of driving clock speeds and straight-line instruction throughput ever higher, they are instead turning en masse to hyperthreading and multicore architectures. Both of these features are already available on chips today; in particular, multicore is available on current PowerPC and Sparc IV processors, and is coming in 2005 from Intel and AMD. Indeed, the big theme of the 2004 In-Stat/MDR Fall Processor Forum was multicore devices, as many companies showed new or updated multicore processors. Looking back, it’s not much of a stretch to call 2004 the year of multicore. And that puts us at a fundamental turning point in software development, at least for the next few years and for applications targeting general-purpose desktop computers and low-end servers (which happens to account for the vast bulk of the dollar value of software sold today). In this article, I’ll describe the changing face of hardware, why it suddenly does matter to software, and how specifically the concurrency revolution matters to you and is going to change the way you will likely be writing software in the future. Arguably, the free lunch has already been over for a year or two, only we’re just now noticing.</t>
+  </si>
+  <si>
+    <t>Dr. Dobb's Journal</t>
+  </si>
+  <si>
+    <t>http://www.mscs.mu.edu/~rge/cosc2200/homework-fall2013/Readings/FreeLunchIsOver.pdf</t>
+  </si>
+  <si>
+    <t>Guru of the Week</t>
+  </si>
+  <si>
+    <t>Universiteit van Amsterdam</t>
+  </si>
+  <si>
+    <t>https://research.hva.nl/en/publications/engineering-emergence-applied-theory-for-game-design</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1517,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1435,15 +1804,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W29"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="8.7265625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1473,7 +1845,7 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
@@ -1526,7 +1898,7 @@
       <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
@@ -1538,7 +1910,7 @@
       <c r="G2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L2" t="s">
@@ -1582,7 +1954,7 @@
       <c r="C3" t="s">
         <v>312</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>311</v>
       </c>
       <c r="E3" t="s">
@@ -1597,7 +1969,7 @@
       <c r="H3" t="s">
         <v>317</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>11</v>
       </c>
       <c r="L3" t="s">
@@ -1644,7 +2016,7 @@
       <c r="C4" t="s">
         <v>318</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>319</v>
       </c>
       <c r="E4" t="s">
@@ -1712,7 +2084,7 @@
       <c r="G5" t="s">
         <v>324</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>325</v>
       </c>
       <c r="L5" t="s">
@@ -1768,10 +2140,10 @@
       <c r="G6" t="s">
         <v>334</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>9</v>
       </c>
       <c r="L6" t="s">
@@ -1885,10 +2257,10 @@
       <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>53</v>
       </c>
       <c r="F9" t="s">
@@ -1897,10 +2269,10 @@
       <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="3">
         <v>2</v>
       </c>
       <c r="L9" t="s">
@@ -1947,10 +2319,10 @@
       <c r="G10" t="s">
         <v>58</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>19</v>
       </c>
       <c r="L10" t="s">
@@ -2032,7 +2404,7 @@
       <c r="G12" t="s">
         <v>225</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>339</v>
       </c>
       <c r="L12" t="s">
@@ -2059,7 +2431,7 @@
       <c r="T12" t="s">
         <v>170</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="U12" s="1" t="s">
         <v>340</v>
       </c>
       <c r="V12" t="s">
@@ -2164,7 +2536,7 @@
       <c r="F15" t="s">
         <v>231</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="1" t="s">
         <v>232</v>
       </c>
       <c r="L15" t="s">
@@ -2217,7 +2589,7 @@
       <c r="F16" t="s">
         <v>236</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
         <v>237</v>
       </c>
       <c r="L16" t="s">
@@ -2270,7 +2642,7 @@
       <c r="G17" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>77</v>
       </c>
       <c r="M17" t="s">
@@ -2311,7 +2683,7 @@
       <c r="F18" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>81</v>
       </c>
       <c r="M18" t="s">
@@ -2352,7 +2724,7 @@
       <c r="G19" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>104</v>
       </c>
       <c r="M19" t="s">
@@ -2393,7 +2765,7 @@
       <c r="F20" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>103</v>
       </c>
       <c r="M20" t="s">
@@ -2415,7 +2787,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3182</v>
       </c>
@@ -2437,10 +2809,10 @@
       <c r="G21" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="3">
         <v>12</v>
       </c>
       <c r="M21" t="s">
@@ -2467,25 +2839,22 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>3245</v>
+        <v>3097</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>111</v>
+        <v>176</v>
+      </c>
+      <c r="D22" t="s">
+        <v>242</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>243</v>
       </c>
       <c r="G22" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>110</v>
+        <v>244</v>
       </c>
       <c r="M22" t="s">
         <v>27</v>
@@ -2500,39 +2869,36 @@
         <v>52</v>
       </c>
       <c r="S22">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="T22" t="s">
-        <v>106</v>
-      </c>
-      <c r="V22" t="s">
-        <v>109</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>3255</v>
+        <v>3120</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>120</v>
+        <v>177</v>
+      </c>
+      <c r="D23" t="s">
+        <v>342</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>345</v>
       </c>
       <c r="G23" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>117</v>
+        <v>343</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J23" s="3">
+        <v>20</v>
       </c>
       <c r="M23" t="s">
         <v>27</v>
@@ -2547,36 +2913,36 @@
         <v>52</v>
       </c>
       <c r="S23">
-        <v>2009</v>
+        <v>2014</v>
       </c>
       <c r="T23" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="V23" t="s">
-        <v>116</v>
+        <v>346</v>
+      </c>
+      <c r="W23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>3269</v>
+        <v>3126</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>123</v>
+        <v>178</v>
+      </c>
+      <c r="D24" t="s">
+        <v>247</v>
       </c>
       <c r="F24" t="s">
-        <v>127</v>
+        <v>248</v>
       </c>
       <c r="G24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H24" t="s">
-        <v>124</v>
+        <v>249</v>
       </c>
       <c r="M24" t="s">
         <v>27</v>
@@ -2591,42 +2957,36 @@
         <v>52</v>
       </c>
       <c r="S24">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="T24" t="s">
-        <v>121</v>
-      </c>
-      <c r="V24" t="s">
-        <v>126</v>
-      </c>
-      <c r="W24" t="s">
-        <v>73</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>3284</v>
+        <v>3132</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>133</v>
+        <v>179</v>
+      </c>
+      <c r="D25" t="s">
+        <v>250</v>
+      </c>
+      <c r="E25" t="s">
+        <v>349</v>
       </c>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>348</v>
       </c>
       <c r="G25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>135</v>
+        <v>252</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="M25" t="s">
         <v>27</v>
@@ -2641,36 +3001,39 @@
         <v>52</v>
       </c>
       <c r="S25">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="T25" t="s">
-        <v>128</v>
+        <v>179</v>
+      </c>
+      <c r="V25" t="s">
+        <v>72</v>
+      </c>
+      <c r="W25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>3325</v>
+        <v>3162</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>141</v>
+        <v>180</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="F26" t="s">
-        <v>142</v>
+        <v>352</v>
       </c>
       <c r="G26" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>139</v>
+        <v>255</v>
+      </c>
+      <c r="H26" t="s">
+        <v>350</v>
       </c>
       <c r="M26" t="s">
         <v>27</v>
@@ -2685,36 +3048,45 @@
         <v>52</v>
       </c>
       <c r="S26">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="T26" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="V26" t="s">
-        <v>143</v>
+        <v>72</v>
+      </c>
+      <c r="W26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>3343</v>
+        <v>3179</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>148</v>
+        <v>181</v>
+      </c>
+      <c r="D27" t="s">
+        <v>354</v>
+      </c>
+      <c r="E27" t="s">
+        <v>353</v>
       </c>
       <c r="F27" t="s">
-        <v>145</v>
+        <v>257</v>
       </c>
       <c r="G27" t="s">
-        <v>146</v>
-      </c>
-      <c r="H27" t="s">
-        <v>149</v>
+        <v>258</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>355</v>
       </c>
       <c r="M27" t="s">
         <v>27</v>
@@ -2729,39 +3101,36 @@
         <v>52</v>
       </c>
       <c r="S27">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="T27" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="V27" t="s">
-        <v>72</v>
-      </c>
-      <c r="W27" t="s">
-        <v>73</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>3359</v>
+        <v>3245</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="F28" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="G28" t="s">
-        <v>156</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>153</v>
+        <v>109</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="M28" t="s">
         <v>27</v>
@@ -2776,66 +3145,1352 @@
         <v>52</v>
       </c>
       <c r="S28">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="T28" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="V28" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29">
+        <v>3255</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" t="s">
+        <v>116</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M29" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+      <c r="R29" t="s">
+        <v>52</v>
+      </c>
+      <c r="S29">
+        <v>2009</v>
+      </c>
+      <c r="T29" t="s">
+        <v>113</v>
+      </c>
+      <c r="V29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>3269</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M30" t="s">
+        <v>27</v>
+      </c>
+      <c r="N30" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+      <c r="R30" t="s">
+        <v>52</v>
+      </c>
+      <c r="S30">
+        <v>2010</v>
+      </c>
+      <c r="T30" t="s">
+        <v>121</v>
+      </c>
+      <c r="V30" t="s">
+        <v>126</v>
+      </c>
+      <c r="W30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>3284</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" t="s">
+        <v>131</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M31" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+      <c r="R31" t="s">
+        <v>52</v>
+      </c>
+      <c r="S31">
+        <v>2010</v>
+      </c>
+      <c r="T31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>3298</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>357</v>
+      </c>
+      <c r="D32" t="s">
+        <v>358</v>
+      </c>
+      <c r="E32" t="s">
+        <v>359</v>
+      </c>
+      <c r="F32" t="s">
+        <v>360</v>
+      </c>
+      <c r="G32" t="s">
+        <v>361</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="M32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q32">
+        <v>2</v>
+      </c>
+      <c r="R32" t="s">
+        <v>52</v>
+      </c>
+      <c r="S32">
+        <v>2011</v>
+      </c>
+      <c r="T32" t="s">
+        <v>182</v>
+      </c>
+      <c r="V32" t="s">
+        <v>72</v>
+      </c>
+      <c r="W32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>3308</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>365</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F33" t="s">
+        <v>367</v>
+      </c>
+      <c r="G33" t="s">
+        <v>264</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="M33" t="s">
+        <v>27</v>
+      </c>
+      <c r="N33" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33" t="s">
+        <v>52</v>
+      </c>
+      <c r="S33">
+        <v>2012</v>
+      </c>
+      <c r="T33" t="s">
+        <v>183</v>
+      </c>
+      <c r="V33" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>3323</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" t="s">
+        <v>373</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F34" t="s">
+        <v>266</v>
+      </c>
+      <c r="G34" t="s">
+        <v>267</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="M34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N34" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q34">
+        <v>2</v>
+      </c>
+      <c r="R34" t="s">
+        <v>52</v>
+      </c>
+      <c r="S34">
+        <v>2009</v>
+      </c>
+      <c r="T34" t="s">
+        <v>184</v>
+      </c>
+      <c r="U34" t="s">
+        <v>371</v>
+      </c>
+      <c r="V34" t="s">
+        <v>370</v>
+      </c>
+      <c r="W34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>3325</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" t="s">
+        <v>143</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M35" t="s">
+        <v>27</v>
+      </c>
+      <c r="N35" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q35">
+        <v>2</v>
+      </c>
+      <c r="R35" t="s">
+        <v>52</v>
+      </c>
+      <c r="S35">
+        <v>2015</v>
+      </c>
+      <c r="T35" t="s">
+        <v>136</v>
+      </c>
+      <c r="V35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3329</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>376</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F36" t="s">
+        <v>381</v>
+      </c>
+      <c r="G36" t="s">
+        <v>379</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="J36">
+        <v>12</v>
+      </c>
+      <c r="M36" t="s">
+        <v>27</v>
+      </c>
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q36">
+        <v>2</v>
+      </c>
+      <c r="R36" t="s">
+        <v>52</v>
+      </c>
+      <c r="S36">
+        <v>2010</v>
+      </c>
+      <c r="T36" t="s">
+        <v>185</v>
+      </c>
+      <c r="V36" t="s">
+        <v>382</v>
+      </c>
+      <c r="W36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>3335</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F37" t="s">
+        <v>385</v>
+      </c>
+      <c r="G37" t="s">
+        <v>272</v>
+      </c>
+      <c r="J37"/>
+      <c r="M37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N37" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37" t="s">
+        <v>52</v>
+      </c>
+      <c r="S37">
+        <v>2010</v>
+      </c>
+      <c r="T37" t="s">
+        <v>186</v>
+      </c>
+      <c r="U37" t="s">
+        <v>383</v>
+      </c>
+      <c r="V37" t="s">
+        <v>384</v>
+      </c>
+      <c r="W37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>3343</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" t="s">
+        <v>149</v>
+      </c>
+      <c r="M38" t="s">
+        <v>27</v>
+      </c>
+      <c r="N38" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q38">
+        <v>2</v>
+      </c>
+      <c r="R38" t="s">
+        <v>52</v>
+      </c>
+      <c r="S38">
+        <v>2011</v>
+      </c>
+      <c r="T38" t="s">
+        <v>144</v>
+      </c>
+      <c r="V38" t="s">
+        <v>72</v>
+      </c>
+      <c r="W38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>3357</v>
+      </c>
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>187</v>
+      </c>
+      <c r="F39" t="s">
+        <v>274</v>
+      </c>
+      <c r="J39"/>
+      <c r="M39" t="s">
+        <v>27</v>
+      </c>
+      <c r="N39" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q39">
+        <v>2</v>
+      </c>
+      <c r="R39" t="s">
+        <v>52</v>
+      </c>
+      <c r="T39" t="s">
+        <v>187</v>
+      </c>
+      <c r="V39" t="s">
+        <v>72</v>
+      </c>
+      <c r="W39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>3358</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>389</v>
+      </c>
+      <c r="D40" t="s">
+        <v>388</v>
+      </c>
+      <c r="E40" t="s">
+        <v>387</v>
+      </c>
+      <c r="F40" t="s">
+        <v>277</v>
+      </c>
+      <c r="G40" t="s">
+        <v>390</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="J40"/>
+      <c r="K40" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="M40" t="s">
+        <v>27</v>
+      </c>
+      <c r="N40" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q40">
+        <v>2</v>
+      </c>
+      <c r="R40" t="s">
+        <v>52</v>
+      </c>
+      <c r="S40">
+        <v>2012</v>
+      </c>
+      <c r="T40" t="s">
+        <v>188</v>
+      </c>
+      <c r="W40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>3359</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" t="s">
+        <v>154</v>
+      </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
+      <c r="G41" t="s">
+        <v>156</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M41" t="s">
+        <v>27</v>
+      </c>
+      <c r="N41" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41" t="s">
+        <v>52</v>
+      </c>
+      <c r="S41">
+        <v>2016</v>
+      </c>
+      <c r="T41" t="s">
+        <v>150</v>
+      </c>
+      <c r="V41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>3369</v>
       </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s">
         <v>162</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D42" t="s">
         <v>163</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E42" t="s">
         <v>164</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F42" t="s">
         <v>159</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G42" t="s">
         <v>161</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H42" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="M29" t="s">
-        <v>27</v>
-      </c>
-      <c r="N29" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q29">
-        <v>2</v>
-      </c>
-      <c r="R29" t="s">
-        <v>52</v>
-      </c>
-      <c r="S29">
+      <c r="M42" t="s">
+        <v>27</v>
+      </c>
+      <c r="N42" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q42">
+        <v>2</v>
+      </c>
+      <c r="R42" t="s">
+        <v>52</v>
+      </c>
+      <c r="S42">
         <v>2013</v>
       </c>
-      <c r="T29" t="s">
+      <c r="T42" t="s">
         <v>158</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V42" t="s">
         <v>161</v>
       </c>
     </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>3411</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>394</v>
+      </c>
+      <c r="D43" t="s">
+        <v>395</v>
+      </c>
+      <c r="F43" t="s">
+        <v>280</v>
+      </c>
+      <c r="G43" t="s">
+        <v>398</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="J43"/>
+      <c r="M43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q43">
+        <v>2</v>
+      </c>
+      <c r="R43" t="s">
+        <v>52</v>
+      </c>
+      <c r="S43">
+        <v>2010</v>
+      </c>
+      <c r="T43" t="s">
+        <v>189</v>
+      </c>
+      <c r="U43" t="s">
+        <v>396</v>
+      </c>
+      <c r="V43" t="s">
+        <v>397</v>
+      </c>
+      <c r="W43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>3427</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>399</v>
+      </c>
+      <c r="D44" t="s">
+        <v>400</v>
+      </c>
+      <c r="E44" t="s">
+        <v>401</v>
+      </c>
+      <c r="F44" t="s">
+        <v>402</v>
+      </c>
+      <c r="G44" t="s">
+        <v>403</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="J44"/>
+      <c r="M44" t="s">
+        <v>27</v>
+      </c>
+      <c r="N44" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q44">
+        <v>2</v>
+      </c>
+      <c r="R44" t="s">
+        <v>52</v>
+      </c>
+      <c r="S44">
+        <v>2012</v>
+      </c>
+      <c r="T44" t="s">
+        <v>190</v>
+      </c>
+      <c r="V44" t="s">
+        <v>329</v>
+      </c>
+      <c r="W44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>3441</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>191</v>
+      </c>
+      <c r="D45" t="s">
+        <v>405</v>
+      </c>
+      <c r="F45" t="s">
+        <v>286</v>
+      </c>
+      <c r="G45" t="s">
+        <v>406</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="J45"/>
+      <c r="M45" t="s">
+        <v>27</v>
+      </c>
+      <c r="N45" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q45">
+        <v>2</v>
+      </c>
+      <c r="R45" t="s">
+        <v>52</v>
+      </c>
+      <c r="S45">
+        <v>2015</v>
+      </c>
+      <c r="T45" t="s">
+        <v>191</v>
+      </c>
+      <c r="V45" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>3469</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="F46" t="s">
+        <v>410</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="J46">
+        <v>96</v>
+      </c>
+      <c r="M46" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q46">
+        <v>2</v>
+      </c>
+      <c r="R46" t="s">
+        <v>52</v>
+      </c>
+      <c r="S46">
+        <v>2016</v>
+      </c>
+      <c r="T46" t="s">
+        <v>192</v>
+      </c>
+      <c r="V46" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>3477</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>193</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F47" t="s">
+        <v>415</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="J47"/>
+      <c r="M47" t="s">
+        <v>27</v>
+      </c>
+      <c r="N47" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q47">
+        <v>2</v>
+      </c>
+      <c r="R47" t="s">
+        <v>52</v>
+      </c>
+      <c r="S47">
+        <v>2010</v>
+      </c>
+      <c r="T47" t="s">
+        <v>193</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="V47" t="s">
+        <v>416</v>
+      </c>
+      <c r="W47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>3496</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" t="s">
+        <v>417</v>
+      </c>
+      <c r="D48" t="s">
+        <v>423</v>
+      </c>
+      <c r="E48" t="s">
+        <v>422</v>
+      </c>
+      <c r="F48" t="s">
+        <v>420</v>
+      </c>
+      <c r="G48" t="s">
+        <v>421</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="J48" t="s">
+        <v>424</v>
+      </c>
+      <c r="M48" t="s">
+        <v>34</v>
+      </c>
+      <c r="N48" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q48">
+        <v>2</v>
+      </c>
+      <c r="R48" t="s">
+        <v>52</v>
+      </c>
+      <c r="S48">
+        <v>2013</v>
+      </c>
+      <c r="T48" t="s">
+        <v>194</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="V48" t="s">
+        <v>426</v>
+      </c>
+      <c r="W48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>3512</v>
+      </c>
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>427</v>
+      </c>
+      <c r="D49" t="s">
+        <v>428</v>
+      </c>
+      <c r="F49" t="s">
+        <v>431</v>
+      </c>
+      <c r="G49" t="s">
+        <v>295</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J49"/>
+      <c r="M49" t="s">
+        <v>27</v>
+      </c>
+      <c r="N49" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q49">
+        <v>2</v>
+      </c>
+      <c r="R49" t="s">
+        <v>52</v>
+      </c>
+      <c r="S49">
+        <v>2013</v>
+      </c>
+      <c r="T49" t="s">
+        <v>195</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="V49" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>3515</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" t="s">
+        <v>432</v>
+      </c>
+      <c r="E50" t="s">
+        <v>433</v>
+      </c>
+      <c r="F50" t="s">
+        <v>434</v>
+      </c>
+      <c r="G50" t="s">
+        <v>436</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="J50">
+        <v>6</v>
+      </c>
+      <c r="M50" t="s">
+        <v>27</v>
+      </c>
+      <c r="N50" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q50">
+        <v>2</v>
+      </c>
+      <c r="R50" t="s">
+        <v>52</v>
+      </c>
+      <c r="S50">
+        <v>2016</v>
+      </c>
+      <c r="T50" t="s">
+        <v>196</v>
+      </c>
+      <c r="V50" t="s">
+        <v>437</v>
+      </c>
+      <c r="W50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>3517</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>438</v>
+      </c>
+      <c r="D51" t="s">
+        <v>446</v>
+      </c>
+      <c r="F51" t="s">
+        <v>440</v>
+      </c>
+      <c r="G51" t="s">
+        <v>300</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="J51">
+        <v>185</v>
+      </c>
+      <c r="M51" t="s">
+        <v>27</v>
+      </c>
+      <c r="N51" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q51">
+        <v>2</v>
+      </c>
+      <c r="R51" t="s">
+        <v>52</v>
+      </c>
+      <c r="S51">
+        <v>2015</v>
+      </c>
+      <c r="T51" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>3529</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" t="s">
+        <v>198</v>
+      </c>
+      <c r="D52" t="s">
+        <v>441</v>
+      </c>
+      <c r="F52" t="s">
+        <v>301</v>
+      </c>
+      <c r="G52" t="s">
+        <v>302</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="J52" t="s">
+        <v>443</v>
+      </c>
+      <c r="M52" t="s">
+        <v>27</v>
+      </c>
+      <c r="N52" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q52">
+        <v>2</v>
+      </c>
+      <c r="R52" t="s">
+        <v>52</v>
+      </c>
+      <c r="S52">
+        <v>2013</v>
+      </c>
+      <c r="T52" t="s">
+        <v>198</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="V52" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>3531</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>448</v>
+      </c>
+      <c r="D53" t="s">
+        <v>449</v>
+      </c>
+      <c r="F53" t="s">
+        <v>450</v>
+      </c>
+      <c r="G53" t="s">
+        <v>304</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="J53"/>
+      <c r="M53" t="s">
+        <v>27</v>
+      </c>
+      <c r="N53" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q53">
+        <v>2</v>
+      </c>
+      <c r="R53" t="s">
+        <v>52</v>
+      </c>
+      <c r="S53">
+        <v>2010</v>
+      </c>
+      <c r="T53" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>3533</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D54" t="s">
+        <v>451</v>
+      </c>
+      <c r="F54" t="s">
+        <v>306</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="J54"/>
+      <c r="M54" t="s">
+        <v>27</v>
+      </c>
+      <c r="N54" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q54">
+        <v>2</v>
+      </c>
+      <c r="R54" t="s">
+        <v>52</v>
+      </c>
+      <c r="S54">
+        <v>2012</v>
+      </c>
+      <c r="T54" t="s">
+        <v>200</v>
+      </c>
+      <c r="V54" t="s">
+        <v>457</v>
+      </c>
+      <c r="W54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>3558</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55" t="s">
+        <v>308</v>
+      </c>
+      <c r="G55" t="s">
+        <v>309</v>
+      </c>
+      <c r="J55"/>
+      <c r="M55" t="s">
+        <v>27</v>
+      </c>
+      <c r="N55" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q55">
+        <v>2</v>
+      </c>
+      <c r="R55" t="s">
+        <v>52</v>
+      </c>
+      <c r="S55">
+        <v>2009</v>
+      </c>
+      <c r="T55" t="s">
+        <v>341</v>
+      </c>
+      <c r="W55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>3562</v>
+      </c>
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" t="s">
+        <v>452</v>
+      </c>
+      <c r="D56" t="s">
+        <v>453</v>
+      </c>
+      <c r="F56" t="s">
+        <v>310</v>
+      </c>
+      <c r="G56" t="s">
+        <v>454</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="J56">
+        <v>8</v>
+      </c>
+      <c r="M56" t="s">
+        <v>27</v>
+      </c>
+      <c r="N56" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q56">
+        <v>2</v>
+      </c>
+      <c r="R56" t="s">
+        <v>52</v>
+      </c>
+      <c r="S56">
+        <v>2013</v>
+      </c>
+      <c r="T56" t="s">
+        <v>202</v>
+      </c>
+      <c r="V56" t="s">
+        <v>456</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:W29" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W29">
-      <sortCondition ref="A1:A29"/>
+  <autoFilter ref="A1:W42" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W42">
+      <sortCondition ref="A1:A42"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -2846,18 +4501,47 @@
     <hyperlink ref="H21" r:id="rId5" xr:uid="{A1CA4A2A-DF85-4017-9070-F32672BF8132}"/>
     <hyperlink ref="H20" r:id="rId6" xr:uid="{51AB7AE4-AEB7-4D74-B586-022575CDE14A}"/>
     <hyperlink ref="H19" r:id="rId7" xr:uid="{AB51E0FE-97CF-4900-836F-DD0B847CBFAE}"/>
-    <hyperlink ref="H22" r:id="rId8" xr:uid="{FFD7FB2D-091C-4A09-9E2D-D1AF69F3FB5D}"/>
-    <hyperlink ref="H25" r:id="rId9" xr:uid="{E3C99D68-C49C-4E39-B459-4A5813A43F01}"/>
-    <hyperlink ref="H26" r:id="rId10" display="https://d1wqtxts1xzle7.cloudfront.net/36637147/SDLC-libre.pdf?1423940228=&amp;response-content-disposition=inline%3B+filename%3DA_Comparison_Between_Three_SDLC_Models_W.pdf&amp;Expires=1726161820&amp;Signature=XHYZ~fSliY2iGbyADM8YvfpjPPO2-V5aoJz2PmsWeR6uL3xwPpflzV1tpCD7xdYqFbu76L6HIti5db0D9ZDMcqHIv9LMiTgM4kWkUhp1MePWsj3~2Hg~mi3fMmv~yiYEbskKsqnwazDIDpJdhEDctVeZ5fG8Ecz-2U~LnTBTmvvpGk~cW5ua8GpKuyWdKTcEEKnI~jfqCE-DiPsW2D4I0i19JGmQbRgFe-cURjeoYJO57XzY7J-jHy2ylKQ0LxSkGvHyDECOVKagc7ZWfTKEIsYWgGb7pLpT1XNwkFk~RVE8egQ0VMxl3JexrTjyMTAuCSxZPdOApes7KZGJGz8iaA__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA" xr:uid="{8C0B7711-2037-4CE2-87A2-584A83054097}"/>
-    <hyperlink ref="H28" r:id="rId11" xr:uid="{C890C6AF-9FD6-49EC-A078-1A1644F9566A}"/>
-    <hyperlink ref="H29" r:id="rId12" xr:uid="{7D0EC0EB-CE95-45A2-9CF8-65E9CA78ECEA}"/>
+    <hyperlink ref="H28" r:id="rId8" xr:uid="{FFD7FB2D-091C-4A09-9E2D-D1AF69F3FB5D}"/>
+    <hyperlink ref="H31" r:id="rId9" xr:uid="{E3C99D68-C49C-4E39-B459-4A5813A43F01}"/>
+    <hyperlink ref="H35" r:id="rId10" display="https://d1wqtxts1xzle7.cloudfront.net/36637147/SDLC-libre.pdf?1423940228=&amp;response-content-disposition=inline%3B+filename%3DA_Comparison_Between_Three_SDLC_Models_W.pdf&amp;Expires=1726161820&amp;Signature=XHYZ~fSliY2iGbyADM8YvfpjPPO2-V5aoJz2PmsWeR6uL3xwPpflzV1tpCD7xdYqFbu76L6HIti5db0D9ZDMcqHIv9LMiTgM4kWkUhp1MePWsj3~2Hg~mi3fMmv~yiYEbskKsqnwazDIDpJdhEDctVeZ5fG8Ecz-2U~LnTBTmvvpGk~cW5ua8GpKuyWdKTcEEKnI~jfqCE-DiPsW2D4I0i19JGmQbRgFe-cURjeoYJO57XzY7J-jHy2ylKQ0LxSkGvHyDECOVKagc7ZWfTKEIsYWgGb7pLpT1XNwkFk~RVE8egQ0VMxl3JexrTjyMTAuCSxZPdOApes7KZGJGz8iaA__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA" xr:uid="{8C0B7711-2037-4CE2-87A2-584A83054097}"/>
+    <hyperlink ref="H41" r:id="rId11" xr:uid="{C890C6AF-9FD6-49EC-A078-1A1644F9566A}"/>
+    <hyperlink ref="H42" r:id="rId12" xr:uid="{7D0EC0EB-CE95-45A2-9CF8-65E9CA78ECEA}"/>
     <hyperlink ref="H5" r:id="rId13" xr:uid="{655C8E9D-B018-447A-8DF1-B08EC0872506}"/>
     <hyperlink ref="H6" r:id="rId14" display="https://www.researchgate.net/profile/Carlos-Lara-Alvarez/publication/314163800_Method_for_Game_Development_Driven_by_User-eXperience_a_Study_of_Rework_Productivity_and_Complexity_of_Use/links/59540e95a6fdcc1697893e96/Method-for-Game-Development-Driven-by-User-eXperience-a-Study-of-Rework-Productivity-and-Complexity-of-Use.pdf" xr:uid="{D50C7C4D-27D7-4DE6-AB88-53C804FDFF82}"/>
     <hyperlink ref="H12" r:id="rId15" xr:uid="{2C25B5CC-84D7-4598-8AA6-8A3EF73DBE13}"/>
     <hyperlink ref="U12" r:id="rId16" xr:uid="{2A66DF0D-13AE-4889-BDE7-A24A7F42229F}"/>
+    <hyperlink ref="H10" r:id="rId17" xr:uid="{E76D70C1-86B7-484D-96B2-93FD25EFEAD0}"/>
+    <hyperlink ref="H15" r:id="rId18" xr:uid="{AE9CE664-332B-431D-B3DB-98C664678286}"/>
+    <hyperlink ref="H16" r:id="rId19" xr:uid="{B80D78C7-6CC6-4162-A75C-DB6E3B841971}"/>
+    <hyperlink ref="H30" r:id="rId20" xr:uid="{E4D6D296-7C9B-446C-B959-8ACD14372554}"/>
+    <hyperlink ref="H23" r:id="rId21" xr:uid="{D987E238-CAD2-4BF9-B4A6-99A80721E723}"/>
+    <hyperlink ref="H25" r:id="rId22" xr:uid="{1CCA98E0-58D4-4212-93F7-8E1C57C29AF9}"/>
+    <hyperlink ref="H27" r:id="rId23" xr:uid="{C8E7338D-F98D-472B-8384-98FD27FFAE3E}"/>
+    <hyperlink ref="H32" r:id="rId24" xr:uid="{A36FC3FE-456E-4B24-80FF-0FC585C1F9A8}"/>
+    <hyperlink ref="H33" r:id="rId25" xr:uid="{13063139-4720-4E5A-96F1-9E3FB8B10012}"/>
+    <hyperlink ref="H34" r:id="rId26" xr:uid="{25D88CB1-9C39-4728-A4D1-95F21C4FEA3C}"/>
+    <hyperlink ref="H36" r:id="rId27" display="https://www.researchgate.net/profile/Josef-Wiemeyer/publication/220244895_Comparison_of_a_traditional_and_a_Video_Game_Based_Balance_Training_Program/links/54806fad0cf25b80dd723663/Comparison-of-a-traditional-and-a-Video-Game-Based-Balance-Training-Program.pdf" xr:uid="{14080658-5D9C-4E83-AF17-5860339D3A5B}"/>
+    <hyperlink ref="H40" r:id="rId28" xr:uid="{134D3FE0-5A40-48DE-8E15-EBDBF060E8E4}"/>
+    <hyperlink ref="H43" r:id="rId29" xr:uid="{E970BD92-CF51-45BE-8D62-0790181870C9}"/>
+    <hyperlink ref="H44" r:id="rId30" xr:uid="{FB7393C9-D947-440C-9644-8AC18271C07D}"/>
+    <hyperlink ref="H45" r:id="rId31" xr:uid="{B9D76FA0-E9E8-44AF-98ED-80F4ED116040}"/>
+    <hyperlink ref="H46" r:id="rId32" xr:uid="{2FC89D54-055E-456A-81D5-92FDDE3B39C0}"/>
+    <hyperlink ref="H47" r:id="rId33" xr:uid="{E4AC55F6-3926-4256-83D2-73BBF336395F}"/>
+    <hyperlink ref="H48" r:id="rId34" xr:uid="{2FB56DB0-3A6D-4CD8-8585-EC4454AB5060}"/>
+    <hyperlink ref="U48" r:id="rId35" xr:uid="{BE069F01-17AC-454E-B5F6-E5544237349D}"/>
+    <hyperlink ref="U47" r:id="rId36" xr:uid="{B9DFBA13-EC9B-4EF3-BF8B-E22B47E4E5CE}"/>
+    <hyperlink ref="H49" r:id="rId37" xr:uid="{1775D29D-FD17-40FF-AA06-6CF7A11E936D}"/>
+    <hyperlink ref="U49" r:id="rId38" xr:uid="{0264BED4-6299-4669-AA6D-E63CE8D943D6}"/>
+    <hyperlink ref="H50" r:id="rId39" xr:uid="{7F7BFEE4-35CE-4655-A13D-6445F7275EBA}"/>
+    <hyperlink ref="H51" r:id="rId40" location="v=onepage&amp;q=Software%20in%2030%20Days%3A%20How%20Agile%20Managers%20Beat%20the%20Odds%2C%20Delight%20Their%20Customers%2C%20And%20Leave%20Competitors%20In%20the%20Dust%20-%20The%20Scrum%20Guide&amp;f=false" display="https://books.google.ca/books?hl=en&amp;lr=&amp;id=FSQbYl5HMo8C&amp;oi=fnd&amp;pg=PP11&amp;dq=Software+in+30+Days:+How+Agile+Managers+Beat+the+Odds,+Delight+Their+Customers,+And+Leave+Competitors+In+the+Dust+-+The+Scrum+Guide&amp;ots=V6fElsfP-i&amp;sig=1MZtgdg3yY7QYqedHD2x_gdHmTU#v=onepage&amp;q=Software%20in%2030%20Days%3A%20How%20Agile%20Managers%20Beat%20the%20Odds%2C%20Delight%20Their%20Customers%2C%20And%20Leave%20Competitors%20In%20the%20Dust%20-%20The%20Scrum%20Guide&amp;f=false" xr:uid="{B87D64C3-60AE-4022-BADF-0534EE7A6578}"/>
+    <hyperlink ref="U52" r:id="rId41" xr:uid="{CD75D0CF-870E-4D70-BD5F-3903917416C3}"/>
+    <hyperlink ref="H52" r:id="rId42" xr:uid="{18F81AD3-66E7-42A7-B4FC-C16488060813}"/>
+    <hyperlink ref="H53" r:id="rId43" xr:uid="{C1B5C16F-B261-476F-80EE-BD333292201C}"/>
+    <hyperlink ref="H56" r:id="rId44" xr:uid="{BA7C5E70-66B2-49D1-B571-1689D7711B0B}"/>
+    <hyperlink ref="H54" r:id="rId45" xr:uid="{C86D6285-05CF-40D3-968E-90357ECD4926}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 
@@ -2865,8 +4549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5B6D92-A38D-431B-8CE9-E20521EDD461}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2893,7 +4577,7 @@
       <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L1" t="s">

</xml_diff>